<commit_message>
Kleine Änderungen an Präsentation v2 und Dateianordnung
</commit_message>
<xml_diff>
--- a/Konzepte/Modell_xQuery.xlsx
+++ b/Konzepte/Modell_xQuery.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzobrazzi/Library/Mobile Documents/com~apple~CloudDocs/Uni/TODO/XML_Praktikum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzobrazzi/Library/Mobile Documents/com~apple~CloudDocs/Uni/TODO/XML_Praktikum/Konzepte/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EDD314-4C65-E849-A27C-AEAF7CCBFEE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4DEA8D-CDCE-A241-A704-BE0C4D33237F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E29A009F-95E9-AB48-8487-F3CE771D36BC}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Funktion für Stand und Surrender zusammen</t>
   </si>
   <si>
-    <t>Funktion die einen Spieler grundsätzlich erstellt und in die DB einträgt (mit Namen, Balance, an welchem Sittz er am Tisch sitzt)</t>
-  </si>
-  <si>
     <t>Funktion die einem Spieler Karten zuteilt</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">    ---&gt; wahrscheinlich werden wir noch ein Hilfsmodul implementieren müssen wo alle kleineren Hilfsfunktionen enthalten sind (siehe TicTacToe was vom Übungsleiter hochgeladen wurde Datei 'tictactoe_helper.xqm'</t>
+  </si>
+  <si>
+    <t>Funktion die einen Spieler grundsätzlich erstellt und in die DB einträgt (mit Namen, Balance, an welchem Sitz er am Tisch sitzt)</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
@@ -579,13 +579,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,13 +593,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,123 +607,123 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>